<commit_message>
modified the code to use real gdp growth instaed of nominal gdp.
</commit_message>
<xml_diff>
--- a/data/Policy_shock.xlsx
+++ b/data/Policy_shock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reubenopondo/Data Science/projects/clients/teal-insights/projects/p26-ddu-dashboard/ddu-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2878DB-CD80-7A42-870A-FA4EAE3C8820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2441478A-C610-7F47-B7FE-AA8DD5D533DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>ISO</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Scale</t>
   </si>
   <si>
-    <t>THA</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
     <t>National currency</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
   </si>
   <si>
     <t>Percent change</t>
-  </si>
-  <si>
-    <t>NGDP</t>
   </si>
   <si>
     <t>Gross domestic product, current prices</t>
@@ -165,6 +156,12 @@
   <si>
     <t>You may change values under this section</t>
   </si>
+  <si>
+    <t>NGDP_RPCH</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,6 +303,12 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="TimesNewRomanPSMT"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="36">
@@ -667,7 +670,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -689,6 +692,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1920,9 +1924,9 @@
           <c:spPr>
             <a:ln w="50800" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:prstDash val="sysDot"/>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1996,7 +2000,7 @@
                   <c:v>66.075000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>66.408000000000015</c:v>
+                  <c:v>66.408000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>66.341000000000008</c:v>
@@ -2005,7 +2009,7 @@
                   <c:v>66.201000000000008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>66.061000000000035</c:v>
+                  <c:v>66.061000000000021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,6 +2225,451 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Debt Projection</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart_data!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>General government gross debt- Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart_data!$K$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2029</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart_data!$K$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65.010999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.075000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.408000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.340999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.200999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.061000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2709-DC48-BE82-46CA949049DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart_data!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Policy shock debt projection</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart_data!$K$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2029</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart_data!$K$3:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65.010999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.075000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.408000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.341000000000008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.201000000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.061000000000021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2709-DC48-BE82-46CA949049DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="79112336"/>
+        <c:axId val="79114064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79112336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79114064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79114064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79112336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-KE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2341,6 +2790,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3536,6 +4025,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3966,15 +4958,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1473200</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3994,6 +4986,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21CBD923-0394-E3E1-43A1-83F494936D4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4301,9 +5329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4334,131 +5360,131 @@
         <v>5</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" s="7">
-        <v>13743.48</v>
+        <v>2.5</v>
       </c>
       <c r="H2" s="7">
-        <v>14590.337</v>
+        <v>2.5</v>
       </c>
       <c r="I2" s="7">
-        <v>15488.664000000001</v>
+        <v>2.5</v>
       </c>
       <c r="J2" s="7">
-        <v>16373.343000000001</v>
+        <v>2.5</v>
       </c>
       <c r="K2" s="7">
-        <v>16889.173999999999</v>
+        <v>2.5</v>
       </c>
       <c r="L2" s="7">
-        <v>15661.290999999999</v>
+        <v>2.5</v>
       </c>
       <c r="M2" s="7">
-        <v>16188.611000000001</v>
+        <v>2.5</v>
       </c>
       <c r="N2" s="7">
-        <v>17378.014999999999</v>
+        <v>2.5</v>
       </c>
       <c r="O2" s="7">
-        <v>17922.038</v>
+        <v>2.5</v>
       </c>
       <c r="P2" s="7">
-        <v>18312.914000000001</v>
+        <v>2.5</v>
       </c>
       <c r="Q2" s="7">
-        <v>19099.578000000001</v>
+        <v>2.5</v>
       </c>
       <c r="R2" s="7">
-        <v>19946.315999999999</v>
+        <v>2.5</v>
       </c>
       <c r="S2" s="7">
-        <v>20883.199000000001</v>
+        <v>2.5</v>
       </c>
       <c r="T2" s="7">
-        <v>21854.991000000002</v>
+        <v>2.5</v>
       </c>
       <c r="U2" s="7">
-        <v>22858.188999999998</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>4</v>
@@ -4511,19 +5537,19 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>4</v>
@@ -4587,7 +5613,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4689,15 +5715,15 @@
     <row r="2" spans="1:21">
       <c r="A2" t="str">
         <f>WEO_Data!A2</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B2" t="str">
         <f>WEO_Data!B2</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C2" t="str">
         <f>WEO_Data!C2</f>
-        <v>NGDP</v>
+        <v>NGDP_RPCH</v>
       </c>
       <c r="D2" t="str">
         <f>WEO_Data!D2</f>
@@ -4709,77 +5735,77 @@
       </c>
       <c r="F2" t="str">
         <f>WEO_Data!F2</f>
-        <v>Billions</v>
+        <v>Percent change</v>
       </c>
       <c r="G2">
         <f>WEO_Data!G2</f>
-        <v>13743.48</v>
+        <v>2.5</v>
       </c>
       <c r="H2">
         <f>WEO_Data!H2</f>
-        <v>14590.337</v>
+        <v>2.5</v>
       </c>
       <c r="I2">
         <f>WEO_Data!I2</f>
-        <v>15488.664000000001</v>
+        <v>2.5</v>
       </c>
       <c r="J2">
         <f>WEO_Data!J2</f>
-        <v>16373.343000000001</v>
+        <v>2.5</v>
       </c>
       <c r="K2">
         <f>WEO_Data!K2</f>
-        <v>16889.173999999999</v>
+        <v>2.5</v>
       </c>
       <c r="L2">
         <f>WEO_Data!L2</f>
-        <v>15661.290999999999</v>
+        <v>2.5</v>
       </c>
       <c r="M2">
         <f>WEO_Data!M2</f>
-        <v>16188.611000000001</v>
+        <v>2.5</v>
       </c>
       <c r="N2">
         <f>WEO_Data!N2</f>
-        <v>17378.014999999999</v>
+        <v>2.5</v>
       </c>
       <c r="O2">
         <f>WEO_Data!O2</f>
-        <v>17922.038</v>
+        <v>2.5</v>
       </c>
       <c r="P2">
         <f>WEO_Data!P2</f>
-        <v>18312.914000000001</v>
+        <v>2.5</v>
       </c>
       <c r="Q2">
         <f>WEO_Data!Q2</f>
-        <v>19099.578000000001</v>
+        <v>2.5</v>
       </c>
       <c r="R2">
         <f>WEO_Data!R2</f>
-        <v>19946.315999999999</v>
+        <v>2.5</v>
       </c>
       <c r="S2">
         <f>WEO_Data!S2</f>
-        <v>20883.199000000001</v>
+        <v>2.5</v>
       </c>
       <c r="T2">
         <f>WEO_Data!T2</f>
-        <v>21854.991000000002</v>
+        <v>2.5</v>
       </c>
       <c r="U2">
         <f>WEO_Data!U2</f>
-        <v>22858.188999999998</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="str">
         <f>WEO_Data!A3</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B3" t="str">
         <f>WEO_Data!B3</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C3" t="str">
         <f>WEO_Data!C3</f>
@@ -4861,11 +5887,11 @@
     <row r="4" spans="1:21">
       <c r="A4" t="str">
         <f>WEO_Data!A4</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B4" t="str">
         <f>WEO_Data!B4</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C4" t="str">
         <f>WEO_Data!C4</f>
@@ -4947,23 +5973,23 @@
     <row r="5" spans="1:21">
       <c r="A5" t="str">
         <f>A2</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B5" t="str">
         <f>B2</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ref="G5:U5" si="0">G4*G11/100</f>
@@ -4971,59 +5997,59 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>3.0262904325820132</v>
+        <v>1.4819774166451296</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>3.184219008500027</v>
+        <v>1.6353167193675855</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>3.8388687172622689</v>
+        <v>2.4479637955383264</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>1.8592117521868952</v>
+        <v>1.5885587867480442</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>1.8342445399299416</v>
+        <v>7.2345184959696018</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="0"/>
-        <v>6.1530958181231306</v>
+        <v>5.6121622323957832</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>3.3819748850134634</v>
+        <v>0.49644805269381709</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="0"/>
-        <v>3.1346624523743554</v>
+        <v>2.7337489012260012</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="0"/>
-        <v>2.9126327878004887</v>
+        <v>3.1246979079916577</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="0"/>
-        <v>1.2377301802210363</v>
+        <v>7.8793809893709807E-2</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" si="0"/>
-        <v>1.5711818546684708</v>
+        <v>0.31274323723041031</v>
       </c>
       <c r="S5" s="1">
         <f t="shared" si="0"/>
-        <v>1.5440432338625394</v>
+        <v>0.11950430859234187</v>
       </c>
       <c r="T5" s="1">
         <f t="shared" si="0"/>
-        <v>1.4431358762989126</v>
+        <v>5.1216688397814424E-2</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" si="0"/>
-        <v>1.4094239458130284</v>
+        <v>6.1020681711754891E-2</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -5118,90 +6144,93 @@
     <row r="8" spans="1:21">
       <c r="A8" t="str">
         <f>A2</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B8" t="str">
         <f>B2</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <f>G2</f>
+        <v>2.5</v>
+      </c>
       <c r="H8" s="4">
-        <f t="shared" ref="H8:U8" si="1">(H2/G2-1)*100</f>
-        <v>6.1618818523401675</v>
+        <f t="shared" ref="H8:U8" si="1">H2</f>
+        <v>2.5</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="1"/>
-        <v>6.156999663544438</v>
+        <v>2.5</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="1"/>
-        <v>5.7117837923270853</v>
+        <v>2.5</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="1"/>
-        <v>3.1504317719356356</v>
+        <v>2.5</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-7.2702371353388866</v>
+        <v>2.5</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="1"/>
-        <v>3.3670276607465022</v>
+        <v>2.5</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="1"/>
-        <v>7.3471652385741937</v>
+        <v>2.5</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" si="1"/>
-        <v>3.1305244010895406</v>
+        <v>2.5</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="1"/>
-        <v>2.1809796408198689</v>
+        <v>2.5</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="1"/>
-        <v>4.2956789946154927</v>
+        <v>2.5</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="1"/>
-        <v>4.4332811960557272</v>
+        <v>2.5</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="1"/>
-        <v>4.6970227484614213</v>
+        <v>2.5</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" si="1"/>
-        <v>4.653463293626614</v>
+        <v>2.5</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="1"/>
-        <v>4.5902466855282542</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="str">
         <f>WEO_Data!A3</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B9" t="str">
         <f>WEO_Data!B3</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C9" t="str">
         <f>WEO_Data!C3</f>
@@ -5283,11 +6312,11 @@
     <row r="10" spans="1:21">
       <c r="A10" t="str">
         <f>WEO_Data!A4</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B10" t="str">
         <f>WEO_Data!B4</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C10" t="str">
         <f>WEO_Data!C4</f>
@@ -5369,20 +6398,20 @@
     <row r="11" spans="1:21">
       <c r="A11" t="str">
         <f>A2</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B11" t="str">
         <f>B2</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
@@ -5390,59 +6419,59 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4">
         <f>((1+H8/100)*((H10+H9)/(G10))-1)*100</f>
-        <v>7.2494680382848564</v>
+        <v>3.5500716652177022</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" ref="I11:U11" si="2">((1+I8/100)*((I10+I9)/(H10))-1)*100</f>
-        <v>7.6217602769400816</v>
+        <v>3.9143011139058492</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="2"/>
-        <v>9.1530214283452196</v>
+        <v>5.8366843793384193</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="2"/>
-        <v>4.5277056040398778</v>
+        <v>3.8685892086502305</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="2"/>
-        <v>3.7115429784094323</v>
+        <v>14.638847624382034</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="2"/>
-        <v>10.547501273845295</v>
+        <v>9.6202448401456753</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="2"/>
-        <v>5.5880091289340461</v>
+        <v>0.82027701115927609</v>
       </c>
       <c r="O11" s="4">
         <f t="shared" si="2"/>
-        <v>5.0202793920153033</v>
+        <v>4.3782013152242172</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="2"/>
-        <v>4.480215329406545</v>
+        <v>4.8064141575912656</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>1.8732200987075842</v>
+        <v>0.11924905016074128</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="2"/>
-        <v>2.3659526783948781</v>
+        <v>0.47094211123721585</v>
       </c>
       <c r="S11" s="4">
         <f t="shared" si="2"/>
-        <v>2.3274343676799258</v>
+        <v>0.18013642934586738</v>
       </c>
       <c r="T11" s="4">
         <f t="shared" si="2"/>
-        <v>2.179930629898208</v>
+        <v>7.7365430126152823E-2</v>
       </c>
       <c r="U11" s="4">
         <f t="shared" si="2"/>
-        <v>2.1335189382737596</v>
+        <v>9.2370205888125945E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5458,7 +6487,7 @@
   <dimension ref="A2:W27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5473,7 +6502,7 @@
   <sheetData>
     <row r="2" spans="1:21">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -5585,11 +6614,11 @@
     <row r="5" spans="1:21">
       <c r="A5" t="str">
         <f>Baseline!A8</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B5" t="str">
         <f>Baseline!B8</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C5" t="str">
         <f>Baseline!C8</f>
@@ -5609,73 +6638,73 @@
       </c>
       <c r="G5" s="4">
         <f>Baseline!G8</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H5" s="4">
         <f>Baseline!H8</f>
-        <v>6.1618818523401675</v>
+        <v>2.5</v>
       </c>
       <c r="I5" s="4">
         <f>Baseline!I8</f>
-        <v>6.156999663544438</v>
+        <v>2.5</v>
       </c>
       <c r="J5" s="4">
         <f>Baseline!J8</f>
-        <v>5.7117837923270853</v>
+        <v>2.5</v>
       </c>
       <c r="K5" s="4">
         <f>Baseline!K8</f>
-        <v>3.1504317719356356</v>
+        <v>2.5</v>
       </c>
       <c r="L5" s="4">
         <f>Baseline!L8</f>
-        <v>-7.2702371353388866</v>
+        <v>2.5</v>
       </c>
       <c r="M5" s="4">
         <f>Baseline!M8</f>
-        <v>3.3670276607465022</v>
+        <v>2.5</v>
       </c>
       <c r="N5" s="4">
         <f>Baseline!N8</f>
-        <v>7.3471652385741937</v>
+        <v>2.5</v>
       </c>
       <c r="O5" s="4">
         <f>Baseline!O8</f>
-        <v>3.1305244010895406</v>
+        <v>2.5</v>
       </c>
       <c r="P5" s="4">
         <f>Baseline!P8</f>
-        <v>2.1809796408198689</v>
+        <v>2.5</v>
       </c>
       <c r="Q5" s="4">
         <f>Baseline!Q8</f>
-        <v>4.2956789946154927</v>
+        <v>2.5</v>
       </c>
       <c r="R5" s="4">
         <f>Baseline!R8</f>
-        <v>4.4332811960557272</v>
+        <v>2.5</v>
       </c>
       <c r="S5" s="4">
         <f>Baseline!S8</f>
-        <v>4.6970227484614213</v>
+        <v>2.5</v>
       </c>
       <c r="T5" s="4">
         <f>Baseline!T8</f>
-        <v>4.653463293626614</v>
+        <v>2.5</v>
       </c>
       <c r="U5" s="4">
         <f>Baseline!U8</f>
-        <v>4.5902466855282542</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="str">
         <f>Baseline!A9</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B6" t="str">
         <f>Baseline!B9</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C6" t="str">
         <f>Baseline!C9</f>
@@ -5757,11 +6786,11 @@
     <row r="7" spans="1:21">
       <c r="A7" t="str">
         <f>Baseline!A11</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B7" t="str">
         <f>Baseline!B11</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C7" t="str">
         <f>Baseline!C11</f>
@@ -5785,68 +6814,68 @@
       </c>
       <c r="H7" s="4">
         <f>Baseline!H11</f>
-        <v>7.2494680382848564</v>
+        <v>3.5500716652177022</v>
       </c>
       <c r="I7" s="4">
         <f>Baseline!I11</f>
-        <v>7.6217602769400816</v>
+        <v>3.9143011139058492</v>
       </c>
       <c r="J7" s="4">
         <f>Baseline!J11</f>
-        <v>9.1530214283452196</v>
+        <v>5.8366843793384193</v>
       </c>
       <c r="K7" s="4">
         <f>Baseline!K11</f>
-        <v>4.5277056040398778</v>
+        <v>3.8685892086502305</v>
       </c>
       <c r="L7" s="4">
         <f>Baseline!L11</f>
-        <v>3.7115429784094323</v>
+        <v>14.638847624382034</v>
       </c>
       <c r="M7" s="4">
         <f>Baseline!M11</f>
-        <v>10.547501273845295</v>
+        <v>9.6202448401456753</v>
       </c>
       <c r="N7" s="4">
         <f>Baseline!N11</f>
-        <v>5.5880091289340461</v>
+        <v>0.82027701115927609</v>
       </c>
       <c r="O7" s="4">
         <f>Baseline!O11</f>
-        <v>5.0202793920153033</v>
+        <v>4.3782013152242172</v>
       </c>
       <c r="P7" s="4">
         <f>Baseline!P11</f>
-        <v>4.480215329406545</v>
+        <v>4.8064141575912656</v>
       </c>
       <c r="Q7" s="4">
         <f>Baseline!Q11</f>
-        <v>1.8732200987075842</v>
+        <v>0.11924905016074128</v>
       </c>
       <c r="R7" s="4">
         <f>Baseline!R11</f>
-        <v>2.3659526783948781</v>
+        <v>0.47094211123721585</v>
       </c>
       <c r="S7" s="4">
         <f>Baseline!S11</f>
-        <v>2.3274343676799258</v>
+        <v>0.18013642934586738</v>
       </c>
       <c r="T7" s="4">
         <f>Baseline!T11</f>
-        <v>2.179930629898208</v>
+        <v>7.7365430126152823E-2</v>
       </c>
       <c r="U7" s="4">
         <f>Baseline!U11</f>
-        <v>2.1335189382737596</v>
+        <v>9.2370205888125945E-2</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -5956,11 +6985,11 @@
     <row r="12" spans="1:21">
       <c r="A12" t="str">
         <f>Baseline!A8</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B12" t="str">
         <f>Baseline!B8</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C12" t="str">
         <f>Baseline!C8</f>
@@ -5997,11 +7026,11 @@
     <row r="13" spans="1:21">
       <c r="A13" t="str">
         <f>Baseline!A9</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B13" t="str">
         <f>Baseline!B9</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C13" t="str">
         <f>Baseline!C9</f>
@@ -6038,11 +7067,11 @@
     <row r="14" spans="1:21">
       <c r="A14" t="str">
         <f>Baseline!A11</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B14" t="str">
         <f>Baseline!B11</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C14" t="str">
         <f>Baseline!C11</f>
@@ -6078,7 +7107,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -6190,11 +7219,11 @@
     <row r="19" spans="1:23">
       <c r="A19" t="str">
         <f>Baseline!A8</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B19" t="str">
         <f>Baseline!B8</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C19" t="str">
         <f>Baseline!C8</f>
@@ -6214,34 +7243,34 @@
       </c>
       <c r="Q19" s="4">
         <f>Q5+Q12</f>
-        <v>4.2956789946154927</v>
+        <v>2.5</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" ref="R19:T19" si="0">R5+R12</f>
-        <v>4.4332811960557272</v>
+        <v>2.5</v>
       </c>
       <c r="S19" s="4">
         <f t="shared" si="0"/>
-        <v>4.6970227484614213</v>
+        <v>2.5</v>
       </c>
       <c r="T19" s="4">
         <f t="shared" si="0"/>
-        <v>4.653463293626614</v>
+        <v>2.5</v>
       </c>
       <c r="U19" s="4">
         <f>U5+U12</f>
-        <v>4.5902466855282542</v>
+        <v>2.5</v>
       </c>
       <c r="W19" s="4"/>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="str">
         <f>Baseline!A9</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B20" t="str">
         <f>Baseline!B9</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C20" t="str">
         <f>Baseline!C9</f>
@@ -6283,11 +7312,11 @@
     <row r="21" spans="1:23">
       <c r="A21" t="str">
         <f>Baseline!A11</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B21" t="str">
         <f>Baseline!B11</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C21" t="str">
         <f>Baseline!C11</f>
@@ -6307,28 +7336,28 @@
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="1"/>
-        <v>1.8732200987075842</v>
+        <v>0.11924905016074128</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="1"/>
-        <v>2.3659526783948781</v>
+        <v>0.47094211123721585</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="1"/>
-        <v>2.3274343676799258</v>
+        <v>0.18013642934586738</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="1"/>
-        <v>2.179930629898208</v>
+        <v>7.7365430126152823E-2</v>
       </c>
       <c r="U21" s="4">
         <f t="shared" si="1"/>
-        <v>2.1335189382737596</v>
+        <v>9.2370205888125945E-2</v>
       </c>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -6440,11 +7469,11 @@
     <row r="26" spans="1:23">
       <c r="A26" t="str">
         <f>Baseline!A10</f>
-        <v>THA</v>
+        <v>Code</v>
       </c>
       <c r="B26" t="str">
         <f>Baseline!B10</f>
-        <v>Thailand</v>
+        <v>Country</v>
       </c>
       <c r="C26" t="str">
         <f>Baseline!C10</f>
@@ -6525,7 +7554,7 @@
     </row>
     <row r="27" spans="1:23">
       <c r="D27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P27" s="4">
         <f>P26</f>
@@ -6537,7 +7566,7 @@
       </c>
       <c r="R27" s="4">
         <f t="shared" ref="R27:U27" si="2">(((1+R21/100)/(1+R19/100))*Q27)-R20</f>
-        <v>66.408000000000015</v>
+        <v>66.408000000000001</v>
       </c>
       <c r="S27" s="4">
         <f t="shared" si="2"/>
@@ -6549,7 +7578,7 @@
       </c>
       <c r="U27" s="4">
         <f t="shared" si="2"/>
-        <v>66.061000000000035</v>
+        <v>66.061000000000021</v>
       </c>
     </row>
   </sheetData>
@@ -6565,7 +7594,7 @@
   <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6729,7 +7758,7 @@
       </c>
       <c r="M3" s="4">
         <f>Policy_shock!R27</f>
-        <v>66.408000000000015</v>
+        <v>66.408000000000001</v>
       </c>
       <c r="N3" s="4">
         <f>Policy_shock!S27</f>
@@ -6741,7 +7770,7 @@
       </c>
       <c r="P3" s="4">
         <f>Policy_shock!U27</f>
-        <v>66.061000000000035</v>
+        <v>66.061000000000021</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>

</xml_diff>